<commit_message>
Adding the regions to the ELC-tradematrice
Table for H2 is prepared, but tilde is deleted
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
+++ b/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/SuppXLS/Trades/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="29" documentId="11_B316FB8291D58ACD044D6FC49EA5C1520CCD395F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A274B94E-4097-42E5-92FA-44D3053CCF00}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="16260" windowHeight="7950"/>
+    <workbookView xWindow="-51720" yWindow="5925" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BI" sheetId="5" r:id="rId1"/>
@@ -13,12 +19,23 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
   <si>
     <t>~TradeLinks</t>
   </si>
@@ -45,12 +62,33 @@
   </si>
   <si>
     <t>DKW</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>DKISLBH</t>
+  </si>
+  <si>
+    <t>DKISL1</t>
+  </si>
+  <si>
+    <t>DKISL</t>
+  </si>
+  <si>
+    <t>DKISL3</t>
+  </si>
+  <si>
+    <t>DKISL2</t>
+  </si>
+  <si>
+    <t>den her virker ikke endnu - og det er godt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -137,7 +175,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -145,12 +183,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -192,7 +233,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -225,9 +266,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -260,6 +318,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -435,25 +510,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="C3:E6"/>
+  <dimension ref="C3:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
@@ -463,21 +538,142 @@
       <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C12" s="1"/>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C16" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C17" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C18" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C19" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -486,20 +682,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="C3:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
@@ -516,22 +712,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
@@ -543,39 +739,39 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Small Update on ELC_trade matrice
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
+++ b/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/SuppXLS/Trades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="11_B316FB8291D58ACD044D6FC49EA5C1520CCD395F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A274B94E-4097-42E5-92FA-44D3053CCF00}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_B316FB8291D58ACD044D6FC49EA5C1520CCD395F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B3D1277-CCF1-4285-88F3-CC4DD365B9ED}"/>
   <bookViews>
     <workbookView xWindow="-51720" yWindow="5925" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
   <si>
     <t>~TradeLinks</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>den her virker ikke endnu - og det er godt</t>
+  </si>
+  <si>
+    <t>på et tidspunkt vil øerne også skulle forbindes med hinanden - men det venter jeg lige med</t>
   </si>
 </sst>
 </file>
@@ -515,7 +518,7 @@
   <dimension ref="C3:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -526,6 +529,9 @@
     <row r="3" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C3" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
trade link matrice for hydrogen
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
+++ b/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\Trades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BA4BF6-903A-4EF1-8C1C-A1EA06136B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3BB178-5750-46D0-BF0F-820DA47AFDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16008" yWindow="1212" windowWidth="21012" windowHeight="14256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BI" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="16">
   <si>
     <t>~TradeLinks</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>DKISL2</t>
-  </si>
-  <si>
-    <t>den her virker ikke endnu - og det er godt</t>
   </si>
   <si>
     <t>på et tidspunkt vil øerne også skulle forbindes med hinanden - men det venter jeg lige med</t>
@@ -518,25 +515,25 @@
   <dimension ref="C1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.3">
       <c r="E1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
@@ -559,7 +556,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
@@ -570,7 +567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
@@ -587,7 +584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
@@ -595,7 +592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
@@ -603,7 +600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
@@ -611,7 +608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
@@ -619,13 +616,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C12" s="1"/>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
         <v>9</v>
       </c>
@@ -648,40 +644,64 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="F14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
+      <c r="H15" s="4">
+        <v>1</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C18" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C19" s="3" t="s">
         <v>13</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -696,14 +716,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
@@ -720,22 +740,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
@@ -753,7 +773,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -766,7 +786,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -779,7 +799,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
establish pipes and ship h2 transport
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
+++ b/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3BB178-5750-46D0-BF0F-820DA47AFDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6591CC22-B5CE-4009-8B6F-1235E5310F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16008" yWindow="1212" windowWidth="21012" windowHeight="14256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16356" yWindow="1560" windowWidth="21012" windowHeight="14256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BI" sheetId="5" r:id="rId1"/>
     <sheet name="Uni" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Fueltrade" sheetId="1" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="33">
   <si>
     <t>~TradeLinks</t>
   </si>
@@ -83,13 +83,64 @@
   </si>
   <si>
     <t>på et tidspunkt vil øerne også skulle forbindes med hinanden - men det venter jeg lige med</t>
+  </si>
+  <si>
+    <t>~TradeLinks_DINS</t>
+  </si>
+  <si>
+    <t>Reg1</t>
+  </si>
+  <si>
+    <t>Reg2</t>
+  </si>
+  <si>
+    <t>Comm</t>
+  </si>
+  <si>
+    <t>Comm2</t>
+  </si>
+  <si>
+    <t>Comm1</t>
+  </si>
+  <si>
+    <t>TradeLink</t>
+  </si>
+  <si>
+    <t>Tech</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>TB_H2_DKISLBH_DKE_01</t>
+  </si>
+  <si>
+    <t>TB_H2_DKISLBH_DKE_02</t>
+  </si>
+  <si>
+    <t>TB_H2_DKISL1_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_H2_DKISL1_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_H2_DKISL2_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_H2_DKISL2_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_H2_DKISL3_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_H2_DKISL3_DKW_02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +160,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -515,7 +572,7 @@
   <dimension ref="C1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,9 +674,7 @@
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C12" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
@@ -714,7 +769,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="C3:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -769,12 +826,231 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1"/>
+  <dimension ref="B2:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="7" max="7" width="21.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fix mistake regarding h2 transport
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
+++ b/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01CF0B7-0E47-46C9-A0EE-6189162C98B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1636DC53-CA34-431B-A6E2-44CDF667D8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17052" yWindow="2256" windowWidth="21012" windowHeight="14256" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16704" yWindow="1908" windowWidth="21012" windowHeight="14256" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BI" sheetId="5" r:id="rId1"/>
@@ -832,7 +832,7 @@
   <dimension ref="B2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -882,7 +882,7 @@
         <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G4" t="s">
         <v>26</v>
@@ -905,7 +905,7 @@
         <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G5" t="s">
         <v>27</v>
@@ -928,7 +928,7 @@
         <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
         <v>28</v>
@@ -951,7 +951,7 @@
         <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G7" t="s">
         <v>29</v>
@@ -974,7 +974,7 @@
         <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G8" t="s">
         <v>30</v>
@@ -997,7 +997,7 @@
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G9" t="s">
         <v>31</v>
@@ -1020,7 +1020,7 @@
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G10" t="s">
         <v>32</v>
@@ -1043,7 +1043,7 @@
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G11" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
change from tradelink U to B
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
+++ b/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB818E2-8D5D-4800-955F-D2E34EA7B0E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C2D03A-9ACE-4E28-B327-524F34A6564D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16704" yWindow="1908" windowWidth="21012" windowHeight="14256" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="21000" windowHeight="14220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BI" sheetId="5" r:id="rId1"/>
@@ -109,9 +109,6 @@
     <t>Tech</t>
   </si>
   <si>
-    <t>U</t>
-  </si>
-  <si>
     <t>TB_H2_DKISLBH_DKE_01</t>
   </si>
   <si>
@@ -134,6 +131,9 @@
   </si>
   <si>
     <t>TB_H2_DKISL3_DKW_02</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -829,7 +829,7 @@
   <dimension ref="B2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -882,10 +882,10 @@
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
@@ -905,10 +905,10 @@
         <v>9</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
@@ -928,10 +928,10 @@
         <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
@@ -951,10 +951,10 @@
         <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
@@ -974,10 +974,10 @@
         <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
@@ -997,10 +997,10 @@
         <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H9" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
@@ -1020,10 +1020,10 @@
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
@@ -1043,10 +1043,10 @@
         <v>9</v>
       </c>
       <c r="G11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" t="s">
         <v>32</v>
-      </c>
-      <c r="H11" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Ammonia, Methanol, Jet Fuel into the Trade Links
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
+++ b/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\Trades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C2D03A-9ACE-4E28-B327-524F34A6564D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45E55A1-117C-40AF-B361-C8760589FF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="21000" windowHeight="14220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1950" windowWidth="38430" windowHeight="10500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BI" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="60">
   <si>
     <t>~TradeLinks</t>
   </si>
@@ -134,6 +134,87 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>MOE</t>
+  </si>
+  <si>
+    <t>KRE</t>
+  </si>
+  <si>
+    <t>TB_MOE_DKISLBH_DKE_01</t>
+  </si>
+  <si>
+    <t>TB_MOE_DKISLBH_DKE_02</t>
+  </si>
+  <si>
+    <t>TB_MOE_DKISL1_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_MOE_DKISL1_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_MOE_DKISL2_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_MOE_DKISL2_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_MOE_DKISL3_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_MOE_DKISL3_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_KRE_DKISLBH_DKE_01</t>
+  </si>
+  <si>
+    <t>TB_KRE_DKISLBH_DKE_02</t>
+  </si>
+  <si>
+    <t>TB_KRE_DKISL1_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_KRE_DKISL1_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_KRE_DKISL2_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_KRE_DKISL2_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_KRE_DKISL3_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_KRE_DKISL3_DKW_02</t>
+  </si>
+  <si>
+    <t>AMM</t>
+  </si>
+  <si>
+    <t>TB_AMM_DKISLBH_DKE_01</t>
+  </si>
+  <si>
+    <t>TB_AMM_DKISLBH_DKE_02</t>
+  </si>
+  <si>
+    <t>TB_AMM_DKISL1_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_AMM_DKISL1_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_AMM_DKISL2_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_AMM_DKISL2_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_AMM_DKISL3_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_AMM_DKISL3_DKW_02</t>
   </si>
 </sst>
 </file>
@@ -575,22 +656,22 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
@@ -613,7 +694,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
@@ -624,7 +705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
@@ -641,7 +722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
@@ -649,7 +730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
@@ -657,7 +738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
@@ -665,7 +746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
@@ -673,10 +754,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>9</v>
       </c>
@@ -699,7 +780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
         <v>7</v>
       </c>
@@ -710,7 +791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
         <v>8</v>
       </c>
@@ -727,7 +808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
@@ -735,7 +816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
         <v>11</v>
       </c>
@@ -743,7 +824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
         <v>12</v>
       </c>
@@ -751,7 +832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
         <v>13</v>
       </c>
@@ -773,14 +854,14 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
@@ -797,22 +878,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
@@ -826,23 +907,23 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B2:H11"/>
+  <dimension ref="B2:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="G12" sqref="G12:G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
@@ -865,7 +946,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -888,7 +969,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -911,7 +992,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -934,7 +1015,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -957,7 +1038,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -980,7 +1061,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -1003,7 +1084,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>13</v>
       </c>
@@ -1026,7 +1107,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -1046,6 +1127,558 @@
         <v>31</v>
       </c>
       <c r="H11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" t="s">
+        <v>45</v>
+      </c>
+      <c r="H22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" t="s">
+        <v>52</v>
+      </c>
+      <c r="H28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" t="s">
+        <v>51</v>
+      </c>
+      <c r="F30" t="s">
+        <v>51</v>
+      </c>
+      <c r="G30" t="s">
+        <v>54</v>
+      </c>
+      <c r="H30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" t="s">
+        <v>51</v>
+      </c>
+      <c r="G31" t="s">
+        <v>55</v>
+      </c>
+      <c r="H31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" t="s">
+        <v>51</v>
+      </c>
+      <c r="F32" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" t="s">
+        <v>56</v>
+      </c>
+      <c r="H32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" t="s">
+        <v>51</v>
+      </c>
+      <c r="F33" t="s">
+        <v>51</v>
+      </c>
+      <c r="G33" t="s">
+        <v>57</v>
+      </c>
+      <c r="H33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" t="s">
+        <v>51</v>
+      </c>
+      <c r="F34" t="s">
+        <v>51</v>
+      </c>
+      <c r="G34" t="s">
+        <v>58</v>
+      </c>
+      <c r="H34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" t="s">
+        <v>51</v>
+      </c>
+      <c r="F35" t="s">
+        <v>51</v>
+      </c>
+      <c r="G35" t="s">
+        <v>59</v>
+      </c>
+      <c r="H35" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1062,7 +1695,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1075,7 +1708,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix B in co2 trade links
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
+++ b/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B959F43A-A5A3-4388-8346-CEA57D241FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AF2E57-AB0E-48AA-B4F6-75B457CF498C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9204" yWindow="2952" windowWidth="30960" windowHeight="12204" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BI" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="69">
   <si>
     <t>~TradeLinks</t>
   </si>
@@ -936,8 +936,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1728,6 +1728,9 @@
       <c r="G36" t="s">
         <v>62</v>
       </c>
+      <c r="H36" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
@@ -1748,6 +1751,9 @@
       <c r="G37" t="s">
         <v>65</v>
       </c>
+      <c r="H37" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
@@ -1768,6 +1774,9 @@
       <c r="G38" t="s">
         <v>63</v>
       </c>
+      <c r="H38" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
@@ -1788,6 +1797,9 @@
       <c r="G39" t="s">
         <v>66</v>
       </c>
+      <c r="H39" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
@@ -1808,6 +1820,9 @@
       <c r="G40" t="s">
         <v>64</v>
       </c>
+      <c r="H40" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
@@ -1828,6 +1843,9 @@
       <c r="G41" t="s">
         <v>67</v>
       </c>
+      <c r="H41" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
@@ -1848,6 +1866,9 @@
       <c r="G42" t="s">
         <v>61</v>
       </c>
+      <c r="H42" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
@@ -1867,6 +1888,9 @@
       </c>
       <c r="G43" t="s">
         <v>68</v>
+      </c>
+      <c r="H43" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>